<commit_message>
Updated IND model - 2025-08-07 10:15
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
+++ b/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBFEDE5D-5F4E-408A-BF18-6F879DC7B2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E16AEAF7-B0A1-4673-9262-97DA2EC5A205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{465BE36B-7B51-47C8-A3AF-A613EC14437E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{A8ECD435-D576-473A-A11E-F1D5D760B31F}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D7DF47-94E6-41BE-B24E-BA5CAD343B37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A66546-0A73-4574-B30A-0EE81A70A917}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7891,7 +7891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83AFF7C-0F7B-40B0-9A14-BF3C50652898}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F761D92-E15F-4C4C-9A15-8D02733C1FED}">
   <dimension ref="A1:U312"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25314,7 +25314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577CBC8B-B081-41DA-9758-704F119404A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1932F5AB-B3CC-47E9-8236-BAFD503AD557}">
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 11:41
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
+++ b/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A87EA5FA-D38C-447D-B9B6-DE67603D4825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15534F74-88BF-49D3-A079-C535349402E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{7D9EC362-5348-4A92-98AF-B3F1DC0EDD41}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{466F2233-2589-4D06-B055-20DF503CDA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FF8AD4-A3F1-404E-BC7E-806A50BF2A01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6116A5CC-C43A-4455-AD5D-0CE4800172DF}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7891,7 +7891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278D0985-8760-4E34-B0A7-D853EAA17C11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB39C576-8283-444C-A2C5-AD6AF47DAE51}">
   <dimension ref="A1:U312"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25314,7 +25314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816CF98D-9A7D-491B-86BF-BB7A2185D4DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF8E90F-2E28-4F8D-BF82-BB7F61944AAA}">
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 12:18
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
+++ b/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F00933F-9139-4B7C-9714-C748C25B68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BE0719F-4576-43A3-B3E0-B61B4DB885A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{76762388-92C8-48CE-975D-E82303DE2731}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{A0E45D63-1E96-4776-B4A3-71583B226E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF758533-4C9B-4D51-9354-F5B7FF7EC10F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA48E227-F1A4-43EE-BF90-743778743739}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7891,7 +7891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77626460-62F1-48F1-8151-7D8226476956}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C924335-DB4E-4B9D-8AB0-3A9AEF93A912}">
   <dimension ref="A1:U312"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25314,7 +25314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B79E57-9E25-4B52-B1FE-55FCF08BD6AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A65850-A517-45E1-B418-BF4FD1BD3A1C}">
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 12:35
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
+++ b/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BE0719F-4576-43A3-B3E0-B61B4DB885A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43F66F3-61E7-455D-9F0C-B46C0C813D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{A0E45D63-1E96-4776-B4A3-71583B226E7D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2DD16053-35EA-4658-8B0F-97419EA1DDE1}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA48E227-F1A4-43EE-BF90-743778743739}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669D6E9D-5DC9-45C5-AC6D-8DA989F26B51}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7891,7 +7891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C924335-DB4E-4B9D-8AB0-3A9AEF93A912}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7836AA-184C-433E-BDDB-218A925EB5A8}">
   <dimension ref="A1:U312"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25314,7 +25314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A65850-A517-45E1-B418-BF4FD1BD3A1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBE702C-EC5E-4D57-B1D2-A3B0BA215202}">
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated IND model - 2025-08-07 12:54
</commit_message>
<xml_diff>
--- a/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
+++ b/VerveStacks_IND/vt_vervestacks_IND_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43F66F3-61E7-455D-9F0C-B46C0C813D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B595056-25AC-4B0D-AEFA-8B0C90639054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2DD16053-35EA-4658-8B0F-97419EA1DDE1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{E45AC91F-03A2-49F5-9B62-5190F018CB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -4903,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669D6E9D-5DC9-45C5-AC6D-8DA989F26B51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29976119-9F1E-4944-8815-9766553BA3F5}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -7891,7 +7891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7836AA-184C-433E-BDDB-218A925EB5A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB4BBE1-C322-4477-96C5-58656A975C1F}">
   <dimension ref="A1:U312"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25314,7 +25314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBE702C-EC5E-4D57-B1D2-A3B0BA215202}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D2B2F6-3097-4E22-A65F-6296469F47C2}">
   <dimension ref="A1:T668"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>